<commit_message>
Updates for Q1 2025
</commit_message>
<xml_diff>
--- a/Apps/YouTubeAnalysis/Analysis/Content/Revenue/Step01a_RevenueByDate.xlsx
+++ b/Apps/YouTubeAnalysis/Analysis/Content/Revenue/Step01a_RevenueByDate.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="10" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2097"/>
+  <dimension ref="A1:B2196"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -16623,7 +16623,7 @@
         <v>45627</v>
       </c>
       <c r="B2067" s="0">
-        <v>48.408999999999999</v>
+        <v>47.694000000000003</v>
       </c>
     </row>
     <row r="2068">
@@ -16631,7 +16631,7 @@
         <v>45628</v>
       </c>
       <c r="B2068" s="0">
-        <v>54.914999999999999</v>
+        <v>53.863999999999997</v>
       </c>
     </row>
     <row r="2069">
@@ -16639,7 +16639,7 @@
         <v>45629</v>
       </c>
       <c r="B2069" s="0">
-        <v>51.920000000000002</v>
+        <v>50.820999999999998</v>
       </c>
     </row>
     <row r="2070">
@@ -16647,7 +16647,7 @@
         <v>45630</v>
       </c>
       <c r="B2070" s="0">
-        <v>48.761000000000003</v>
+        <v>47.479999999999997</v>
       </c>
     </row>
     <row r="2071">
@@ -16655,7 +16655,7 @@
         <v>45631</v>
       </c>
       <c r="B2071" s="0">
-        <v>45.067</v>
+        <v>43.845999999999997</v>
       </c>
     </row>
     <row r="2072">
@@ -16663,7 +16663,7 @@
         <v>45632</v>
       </c>
       <c r="B2072" s="0">
-        <v>56.082999999999998</v>
+        <v>55.304000000000002</v>
       </c>
     </row>
     <row r="2073">
@@ -16671,7 +16671,7 @@
         <v>45633</v>
       </c>
       <c r="B2073" s="0">
-        <v>47.942999999999998</v>
+        <v>46.862000000000002</v>
       </c>
     </row>
     <row r="2074">
@@ -16679,7 +16679,7 @@
         <v>45634</v>
       </c>
       <c r="B2074" s="0">
-        <v>50.561</v>
+        <v>50.054000000000002</v>
       </c>
     </row>
     <row r="2075">
@@ -16687,7 +16687,7 @@
         <v>45635</v>
       </c>
       <c r="B2075" s="0">
-        <v>41.859000000000002</v>
+        <v>40.466000000000001</v>
       </c>
     </row>
     <row r="2076">
@@ -16695,7 +16695,7 @@
         <v>45636</v>
       </c>
       <c r="B2076" s="0">
-        <v>40.646999999999998</v>
+        <v>40.006</v>
       </c>
     </row>
     <row r="2077">
@@ -16703,7 +16703,7 @@
         <v>45637</v>
       </c>
       <c r="B2077" s="0">
-        <v>44.229999999999997</v>
+        <v>42.207000000000001</v>
       </c>
     </row>
     <row r="2078">
@@ -16711,7 +16711,7 @@
         <v>45638</v>
       </c>
       <c r="B2078" s="0">
-        <v>44.438000000000002</v>
+        <v>43.914999999999999</v>
       </c>
     </row>
     <row r="2079">
@@ -16719,7 +16719,7 @@
         <v>45639</v>
       </c>
       <c r="B2079" s="0">
-        <v>40.774999999999999</v>
+        <v>40.317</v>
       </c>
     </row>
     <row r="2080">
@@ -16727,7 +16727,7 @@
         <v>45640</v>
       </c>
       <c r="B2080" s="0">
-        <v>37.152000000000001</v>
+        <v>36.784999999999997</v>
       </c>
     </row>
     <row r="2081">
@@ -16735,7 +16735,7 @@
         <v>45641</v>
       </c>
       <c r="B2081" s="0">
-        <v>41.259999999999998</v>
+        <v>40.831000000000003</v>
       </c>
     </row>
     <row r="2082">
@@ -16743,7 +16743,7 @@
         <v>45642</v>
       </c>
       <c r="B2082" s="0">
-        <v>39.694000000000003</v>
+        <v>38.990000000000002</v>
       </c>
     </row>
     <row r="2083">
@@ -16751,7 +16751,7 @@
         <v>45643</v>
       </c>
       <c r="B2083" s="0">
-        <v>40.505000000000003</v>
+        <v>40.310000000000002</v>
       </c>
     </row>
     <row r="2084">
@@ -16759,7 +16759,7 @@
         <v>45644</v>
       </c>
       <c r="B2084" s="0">
-        <v>36.997</v>
+        <v>36.884</v>
       </c>
     </row>
     <row r="2085">
@@ -16767,7 +16767,7 @@
         <v>45645</v>
       </c>
       <c r="B2085" s="0">
-        <v>37.807000000000002</v>
+        <v>37.57</v>
       </c>
     </row>
     <row r="2086">
@@ -16775,7 +16775,7 @@
         <v>45646</v>
       </c>
       <c r="B2086" s="0">
-        <v>35.643000000000001</v>
+        <v>35.561</v>
       </c>
     </row>
     <row r="2087">
@@ -16783,7 +16783,7 @@
         <v>45647</v>
       </c>
       <c r="B2087" s="0">
-        <v>35.914000000000001</v>
+        <v>35.078000000000003</v>
       </c>
     </row>
     <row r="2088">
@@ -16791,7 +16791,7 @@
         <v>45648</v>
       </c>
       <c r="B2088" s="0">
-        <v>36.68</v>
+        <v>36.427999999999997</v>
       </c>
     </row>
     <row r="2089">
@@ -16799,7 +16799,7 @@
         <v>45649</v>
       </c>
       <c r="B2089" s="0">
-        <v>33.798999999999999</v>
+        <v>33.32</v>
       </c>
     </row>
     <row r="2090">
@@ -16807,7 +16807,7 @@
         <v>45650</v>
       </c>
       <c r="B2090" s="0">
-        <v>27.106000000000002</v>
+        <v>26.841000000000001</v>
       </c>
     </row>
     <row r="2091">
@@ -16815,7 +16815,7 @@
         <v>45651</v>
       </c>
       <c r="B2091" s="0">
-        <v>31.632999999999999</v>
+        <v>31.390000000000001</v>
       </c>
     </row>
     <row r="2092">
@@ -16823,7 +16823,7 @@
         <v>45652</v>
       </c>
       <c r="B2092" s="0">
-        <v>38.466999999999999</v>
+        <v>38.408999999999999</v>
       </c>
     </row>
     <row r="2093">
@@ -16831,7 +16831,7 @@
         <v>45653</v>
       </c>
       <c r="B2093" s="0">
-        <v>34.485999999999997</v>
+        <v>34.167000000000002</v>
       </c>
     </row>
     <row r="2094">
@@ -16839,7 +16839,7 @@
         <v>45654</v>
       </c>
       <c r="B2094" s="0">
-        <v>39.762999999999998</v>
+        <v>39.210999999999999</v>
       </c>
     </row>
     <row r="2095">
@@ -16847,7 +16847,7 @@
         <v>45655</v>
       </c>
       <c r="B2095" s="0">
-        <v>36.366999999999997</v>
+        <v>36.292999999999999</v>
       </c>
     </row>
     <row r="2096">
@@ -16855,7 +16855,7 @@
         <v>45656</v>
       </c>
       <c r="B2096" s="0">
-        <v>38.868000000000002</v>
+        <v>38.896999999999998</v>
       </c>
     </row>
     <row r="2097">
@@ -16863,7 +16863,799 @@
         <v>45657</v>
       </c>
       <c r="B2097" s="0">
-        <v>29.823</v>
+        <v>29.829000000000001</v>
+      </c>
+    </row>
+    <row r="2098">
+      <c r="A2098" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B2098" s="0">
+        <v>23.942</v>
+      </c>
+    </row>
+    <row r="2099">
+      <c r="A2099" s="1">
+        <v>45659</v>
+      </c>
+      <c r="B2099" s="0">
+        <v>31.733000000000001</v>
+      </c>
+    </row>
+    <row r="2100">
+      <c r="A2100" s="1">
+        <v>45660</v>
+      </c>
+      <c r="B2100" s="0">
+        <v>34.335999999999999</v>
+      </c>
+    </row>
+    <row r="2101">
+      <c r="A2101" s="1">
+        <v>45661</v>
+      </c>
+      <c r="B2101" s="0">
+        <v>36.811999999999998</v>
+      </c>
+    </row>
+    <row r="2102">
+      <c r="A2102" s="1">
+        <v>45662</v>
+      </c>
+      <c r="B2102" s="0">
+        <v>32.368000000000002</v>
+      </c>
+    </row>
+    <row r="2103">
+      <c r="A2103" s="1">
+        <v>45663</v>
+      </c>
+      <c r="B2103" s="0">
+        <v>32.813000000000002</v>
+      </c>
+    </row>
+    <row r="2104">
+      <c r="A2104" s="1">
+        <v>45664</v>
+      </c>
+      <c r="B2104" s="0">
+        <v>33.518000000000001</v>
+      </c>
+    </row>
+    <row r="2105">
+      <c r="A2105" s="1">
+        <v>45665</v>
+      </c>
+      <c r="B2105" s="0">
+        <v>39.728000000000002</v>
+      </c>
+    </row>
+    <row r="2106">
+      <c r="A2106" s="1">
+        <v>45666</v>
+      </c>
+      <c r="B2106" s="0">
+        <v>32.076999999999998</v>
+      </c>
+    </row>
+    <row r="2107">
+      <c r="A2107" s="1">
+        <v>45667</v>
+      </c>
+      <c r="B2107" s="0">
+        <v>33.412999999999997</v>
+      </c>
+    </row>
+    <row r="2108">
+      <c r="A2108" s="1">
+        <v>45668</v>
+      </c>
+      <c r="B2108" s="0">
+        <v>32.253</v>
+      </c>
+    </row>
+    <row r="2109">
+      <c r="A2109" s="1">
+        <v>45669</v>
+      </c>
+      <c r="B2109" s="0">
+        <v>30.404</v>
+      </c>
+    </row>
+    <row r="2110">
+      <c r="A2110" s="1">
+        <v>45670</v>
+      </c>
+      <c r="B2110" s="0">
+        <v>31.513000000000002</v>
+      </c>
+    </row>
+    <row r="2111">
+      <c r="A2111" s="1">
+        <v>45671</v>
+      </c>
+      <c r="B2111" s="0">
+        <v>34.921999999999997</v>
+      </c>
+    </row>
+    <row r="2112">
+      <c r="A2112" s="1">
+        <v>45672</v>
+      </c>
+      <c r="B2112" s="0">
+        <v>39.247999999999998</v>
+      </c>
+    </row>
+    <row r="2113">
+      <c r="A2113" s="1">
+        <v>45673</v>
+      </c>
+      <c r="B2113" s="0">
+        <v>32.865000000000002</v>
+      </c>
+    </row>
+    <row r="2114">
+      <c r="A2114" s="1">
+        <v>45674</v>
+      </c>
+      <c r="B2114" s="0">
+        <v>34.598999999999997</v>
+      </c>
+    </row>
+    <row r="2115">
+      <c r="A2115" s="1">
+        <v>45675</v>
+      </c>
+      <c r="B2115" s="0">
+        <v>33.643999999999998</v>
+      </c>
+    </row>
+    <row r="2116">
+      <c r="A2116" s="1">
+        <v>45676</v>
+      </c>
+      <c r="B2116" s="0">
+        <v>33.843000000000004</v>
+      </c>
+    </row>
+    <row r="2117">
+      <c r="A2117" s="1">
+        <v>45677</v>
+      </c>
+      <c r="B2117" s="0">
+        <v>34.415999999999997</v>
+      </c>
+    </row>
+    <row r="2118">
+      <c r="A2118" s="1">
+        <v>45678</v>
+      </c>
+      <c r="B2118" s="0">
+        <v>32.594999999999999</v>
+      </c>
+    </row>
+    <row r="2119">
+      <c r="A2119" s="1">
+        <v>45679</v>
+      </c>
+      <c r="B2119" s="0">
+        <v>37.442</v>
+      </c>
+    </row>
+    <row r="2120">
+      <c r="A2120" s="1">
+        <v>45680</v>
+      </c>
+      <c r="B2120" s="0">
+        <v>33.332999999999998</v>
+      </c>
+    </row>
+    <row r="2121">
+      <c r="A2121" s="1">
+        <v>45681</v>
+      </c>
+      <c r="B2121" s="0">
+        <v>31.885999999999999</v>
+      </c>
+    </row>
+    <row r="2122">
+      <c r="A2122" s="1">
+        <v>45682</v>
+      </c>
+      <c r="B2122" s="0">
+        <v>32.490000000000002</v>
+      </c>
+    </row>
+    <row r="2123">
+      <c r="A2123" s="1">
+        <v>45683</v>
+      </c>
+      <c r="B2123" s="0">
+        <v>35.933999999999997</v>
+      </c>
+    </row>
+    <row r="2124">
+      <c r="A2124" s="1">
+        <v>45684</v>
+      </c>
+      <c r="B2124" s="0">
+        <v>32.494</v>
+      </c>
+    </row>
+    <row r="2125">
+      <c r="A2125" s="1">
+        <v>45685</v>
+      </c>
+      <c r="B2125" s="0">
+        <v>34.848999999999997</v>
+      </c>
+    </row>
+    <row r="2126">
+      <c r="A2126" s="1">
+        <v>45686</v>
+      </c>
+      <c r="B2126" s="0">
+        <v>30.919</v>
+      </c>
+    </row>
+    <row r="2127">
+      <c r="A2127" s="1">
+        <v>45687</v>
+      </c>
+      <c r="B2127" s="0">
+        <v>32.436999999999998</v>
+      </c>
+    </row>
+    <row r="2128">
+      <c r="A2128" s="1">
+        <v>45688</v>
+      </c>
+      <c r="B2128" s="0">
+        <v>30.149999999999999</v>
+      </c>
+    </row>
+    <row r="2129">
+      <c r="A2129" s="1">
+        <v>45689</v>
+      </c>
+      <c r="B2129" s="0">
+        <v>36.502000000000002</v>
+      </c>
+    </row>
+    <row r="2130">
+      <c r="A2130" s="1">
+        <v>45690</v>
+      </c>
+      <c r="B2130" s="0">
+        <v>29.632000000000001</v>
+      </c>
+    </row>
+    <row r="2131">
+      <c r="A2131" s="1">
+        <v>45691</v>
+      </c>
+      <c r="B2131" s="0">
+        <v>33.588000000000001</v>
+      </c>
+    </row>
+    <row r="2132">
+      <c r="A2132" s="1">
+        <v>45692</v>
+      </c>
+      <c r="B2132" s="0">
+        <v>36.162999999999997</v>
+      </c>
+    </row>
+    <row r="2133">
+      <c r="A2133" s="1">
+        <v>45693</v>
+      </c>
+      <c r="B2133" s="0">
+        <v>35.768000000000001</v>
+      </c>
+    </row>
+    <row r="2134">
+      <c r="A2134" s="1">
+        <v>45694</v>
+      </c>
+      <c r="B2134" s="0">
+        <v>35.43</v>
+      </c>
+    </row>
+    <row r="2135">
+      <c r="A2135" s="1">
+        <v>45695</v>
+      </c>
+      <c r="B2135" s="0">
+        <v>30.286000000000001</v>
+      </c>
+    </row>
+    <row r="2136">
+      <c r="A2136" s="1">
+        <v>45696</v>
+      </c>
+      <c r="B2136" s="0">
+        <v>41.018999999999998</v>
+      </c>
+    </row>
+    <row r="2137">
+      <c r="A2137" s="1">
+        <v>45697</v>
+      </c>
+      <c r="B2137" s="0">
+        <v>35.456000000000003</v>
+      </c>
+    </row>
+    <row r="2138">
+      <c r="A2138" s="1">
+        <v>45698</v>
+      </c>
+      <c r="B2138" s="0">
+        <v>37.344000000000001</v>
+      </c>
+    </row>
+    <row r="2139">
+      <c r="A2139" s="1">
+        <v>45699</v>
+      </c>
+      <c r="B2139" s="0">
+        <v>34.341999999999999</v>
+      </c>
+    </row>
+    <row r="2140">
+      <c r="A2140" s="1">
+        <v>45700</v>
+      </c>
+      <c r="B2140" s="0">
+        <v>29.718</v>
+      </c>
+    </row>
+    <row r="2141">
+      <c r="A2141" s="1">
+        <v>45701</v>
+      </c>
+      <c r="B2141" s="0">
+        <v>30.942</v>
+      </c>
+    </row>
+    <row r="2142">
+      <c r="A2142" s="1">
+        <v>45702</v>
+      </c>
+      <c r="B2142" s="0">
+        <v>28.803999999999998</v>
+      </c>
+    </row>
+    <row r="2143">
+      <c r="A2143" s="1">
+        <v>45703</v>
+      </c>
+      <c r="B2143" s="0">
+        <v>30.295000000000002</v>
+      </c>
+    </row>
+    <row r="2144">
+      <c r="A2144" s="1">
+        <v>45704</v>
+      </c>
+      <c r="B2144" s="0">
+        <v>31.785</v>
+      </c>
+    </row>
+    <row r="2145">
+      <c r="A2145" s="1">
+        <v>45705</v>
+      </c>
+      <c r="B2145" s="0">
+        <v>35.765000000000001</v>
+      </c>
+    </row>
+    <row r="2146">
+      <c r="A2146" s="1">
+        <v>45706</v>
+      </c>
+      <c r="B2146" s="0">
+        <v>36.331000000000003</v>
+      </c>
+    </row>
+    <row r="2147">
+      <c r="A2147" s="1">
+        <v>45707</v>
+      </c>
+      <c r="B2147" s="0">
+        <v>37.331000000000003</v>
+      </c>
+    </row>
+    <row r="2148">
+      <c r="A2148" s="1">
+        <v>45708</v>
+      </c>
+      <c r="B2148" s="0">
+        <v>51.691000000000003</v>
+      </c>
+    </row>
+    <row r="2149">
+      <c r="A2149" s="1">
+        <v>45709</v>
+      </c>
+      <c r="B2149" s="0">
+        <v>37.850000000000001</v>
+      </c>
+    </row>
+    <row r="2150">
+      <c r="A2150" s="1">
+        <v>45710</v>
+      </c>
+      <c r="B2150" s="0">
+        <v>37.988999999999997</v>
+      </c>
+    </row>
+    <row r="2151">
+      <c r="A2151" s="1">
+        <v>45711</v>
+      </c>
+      <c r="B2151" s="0">
+        <v>32.676000000000002</v>
+      </c>
+    </row>
+    <row r="2152">
+      <c r="A2152" s="1">
+        <v>45712</v>
+      </c>
+      <c r="B2152" s="0">
+        <v>35.735999999999997</v>
+      </c>
+    </row>
+    <row r="2153">
+      <c r="A2153" s="1">
+        <v>45713</v>
+      </c>
+      <c r="B2153" s="0">
+        <v>33.637999999999998</v>
+      </c>
+    </row>
+    <row r="2154">
+      <c r="A2154" s="1">
+        <v>45714</v>
+      </c>
+      <c r="B2154" s="0">
+        <v>33.860999999999997</v>
+      </c>
+    </row>
+    <row r="2155">
+      <c r="A2155" s="1">
+        <v>45715</v>
+      </c>
+      <c r="B2155" s="0">
+        <v>40.804000000000002</v>
+      </c>
+    </row>
+    <row r="2156">
+      <c r="A2156" s="1">
+        <v>45716</v>
+      </c>
+      <c r="B2156" s="0">
+        <v>26.375</v>
+      </c>
+    </row>
+    <row r="2157">
+      <c r="A2157" s="1">
+        <v>45717</v>
+      </c>
+      <c r="B2157" s="0">
+        <v>30.652000000000001</v>
+      </c>
+    </row>
+    <row r="2158">
+      <c r="A2158" s="1">
+        <v>45718</v>
+      </c>
+      <c r="B2158" s="0">
+        <v>28.622</v>
+      </c>
+    </row>
+    <row r="2159">
+      <c r="A2159" s="1">
+        <v>45719</v>
+      </c>
+      <c r="B2159" s="0">
+        <v>30.337</v>
+      </c>
+    </row>
+    <row r="2160">
+      <c r="A2160" s="1">
+        <v>45720</v>
+      </c>
+      <c r="B2160" s="0">
+        <v>33.668999999999997</v>
+      </c>
+    </row>
+    <row r="2161">
+      <c r="A2161" s="1">
+        <v>45721</v>
+      </c>
+      <c r="B2161" s="0">
+        <v>32.527000000000001</v>
+      </c>
+    </row>
+    <row r="2162">
+      <c r="A2162" s="1">
+        <v>45722</v>
+      </c>
+      <c r="B2162" s="0">
+        <v>30.170000000000002</v>
+      </c>
+    </row>
+    <row r="2163">
+      <c r="A2163" s="1">
+        <v>45723</v>
+      </c>
+      <c r="B2163" s="0">
+        <v>28.047000000000001</v>
+      </c>
+    </row>
+    <row r="2164">
+      <c r="A2164" s="1">
+        <v>45724</v>
+      </c>
+      <c r="B2164" s="0">
+        <v>33.301000000000002</v>
+      </c>
+    </row>
+    <row r="2165">
+      <c r="A2165" s="1">
+        <v>45725</v>
+      </c>
+      <c r="B2165" s="0">
+        <v>34.372</v>
+      </c>
+    </row>
+    <row r="2166">
+      <c r="A2166" s="1">
+        <v>45726</v>
+      </c>
+      <c r="B2166" s="0">
+        <v>36.206000000000003</v>
+      </c>
+    </row>
+    <row r="2167">
+      <c r="A2167" s="1">
+        <v>45727</v>
+      </c>
+      <c r="B2167" s="0">
+        <v>30.620999999999999</v>
+      </c>
+    </row>
+    <row r="2168">
+      <c r="A2168" s="1">
+        <v>45728</v>
+      </c>
+      <c r="B2168" s="0">
+        <v>30.753</v>
+      </c>
+    </row>
+    <row r="2169">
+      <c r="A2169" s="1">
+        <v>45729</v>
+      </c>
+      <c r="B2169" s="0">
+        <v>36.825000000000003</v>
+      </c>
+    </row>
+    <row r="2170">
+      <c r="A2170" s="1">
+        <v>45730</v>
+      </c>
+      <c r="B2170" s="0">
+        <v>31.923999999999999</v>
+      </c>
+    </row>
+    <row r="2171">
+      <c r="A2171" s="1">
+        <v>45731</v>
+      </c>
+      <c r="B2171" s="0">
+        <v>31.504000000000001</v>
+      </c>
+    </row>
+    <row r="2172">
+      <c r="A2172" s="1">
+        <v>45732</v>
+      </c>
+      <c r="B2172" s="0">
+        <v>35.167000000000002</v>
+      </c>
+    </row>
+    <row r="2173">
+      <c r="A2173" s="1">
+        <v>45733</v>
+      </c>
+      <c r="B2173" s="0">
+        <v>35.582999999999998</v>
+      </c>
+    </row>
+    <row r="2174">
+      <c r="A2174" s="1">
+        <v>45734</v>
+      </c>
+      <c r="B2174" s="0">
+        <v>41.896999999999998</v>
+      </c>
+    </row>
+    <row r="2175">
+      <c r="A2175" s="1">
+        <v>45735</v>
+      </c>
+      <c r="B2175" s="0">
+        <v>39.893999999999998</v>
+      </c>
+    </row>
+    <row r="2176">
+      <c r="A2176" s="1">
+        <v>45736</v>
+      </c>
+      <c r="B2176" s="0">
+        <v>38.546999999999997</v>
+      </c>
+    </row>
+    <row r="2177">
+      <c r="A2177" s="1">
+        <v>45737</v>
+      </c>
+      <c r="B2177" s="0">
+        <v>31.507000000000001</v>
+      </c>
+    </row>
+    <row r="2178">
+      <c r="A2178" s="1">
+        <v>45738</v>
+      </c>
+      <c r="B2178" s="0">
+        <v>32.219000000000001</v>
+      </c>
+    </row>
+    <row r="2179">
+      <c r="A2179" s="1">
+        <v>45739</v>
+      </c>
+      <c r="B2179" s="0">
+        <v>37.398000000000003</v>
+      </c>
+    </row>
+    <row r="2180">
+      <c r="A2180" s="1">
+        <v>45740</v>
+      </c>
+      <c r="B2180" s="0">
+        <v>38.186</v>
+      </c>
+    </row>
+    <row r="2181">
+      <c r="A2181" s="1">
+        <v>45741</v>
+      </c>
+      <c r="B2181" s="0">
+        <v>32.442999999999998</v>
+      </c>
+    </row>
+    <row r="2182">
+      <c r="A2182" s="1">
+        <v>45742</v>
+      </c>
+      <c r="B2182" s="0">
+        <v>34.433999999999997</v>
+      </c>
+    </row>
+    <row r="2183">
+      <c r="A2183" s="1">
+        <v>45743</v>
+      </c>
+      <c r="B2183" s="0">
+        <v>34.308999999999997</v>
+      </c>
+    </row>
+    <row r="2184">
+      <c r="A2184" s="1">
+        <v>45744</v>
+      </c>
+      <c r="B2184" s="0">
+        <v>30.533999999999999</v>
+      </c>
+    </row>
+    <row r="2185">
+      <c r="A2185" s="1">
+        <v>45745</v>
+      </c>
+      <c r="B2185" s="0">
+        <v>31.523</v>
+      </c>
+    </row>
+    <row r="2186">
+      <c r="A2186" s="1">
+        <v>45746</v>
+      </c>
+      <c r="B2186" s="0">
+        <v>32.908999999999999</v>
+      </c>
+    </row>
+    <row r="2187">
+      <c r="A2187" s="1">
+        <v>45747</v>
+      </c>
+      <c r="B2187" s="0">
+        <v>37.603999999999999</v>
+      </c>
+    </row>
+    <row r="2188">
+      <c r="A2188" s="1">
+        <v>45748</v>
+      </c>
+      <c r="B2188" s="0">
+        <v>29.867000000000001</v>
+      </c>
+    </row>
+    <row r="2189">
+      <c r="A2189" s="1">
+        <v>45749</v>
+      </c>
+      <c r="B2189" s="0">
+        <v>33.765999999999998</v>
+      </c>
+    </row>
+    <row r="2190">
+      <c r="A2190" s="1">
+        <v>45750</v>
+      </c>
+      <c r="B2190" s="0">
+        <v>47.497999999999998</v>
+      </c>
+    </row>
+    <row r="2191">
+      <c r="A2191" s="1">
+        <v>45751</v>
+      </c>
+      <c r="B2191" s="0">
+        <v>28.094000000000001</v>
+      </c>
+    </row>
+    <row r="2192">
+      <c r="A2192" s="1">
+        <v>45752</v>
+      </c>
+      <c r="B2192" s="0">
+        <v>33.213999999999999</v>
+      </c>
+    </row>
+    <row r="2193">
+      <c r="A2193" s="1">
+        <v>45753</v>
+      </c>
+      <c r="B2193" s="0">
+        <v>29.373000000000001</v>
+      </c>
+    </row>
+    <row r="2194">
+      <c r="A2194" s="1">
+        <v>45754</v>
+      </c>
+      <c r="B2194" s="0">
+        <v>39.573999999999998</v>
+      </c>
+    </row>
+    <row r="2195">
+      <c r="A2195" s="1">
+        <v>45755</v>
+      </c>
+      <c r="B2195" s="0">
+        <v>41.936</v>
+      </c>
+    </row>
+    <row r="2196">
+      <c r="A2196" s="1">
+        <v>45756</v>
+      </c>
+      <c r="B2196" s="0">
+        <v>30.515000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>